<commit_message>
Add user service code.
</commit_message>
<xml_diff>
--- a/doc/后续工作20130921起/28分析软件后续工作和服务器站点【持续更新】.xlsx
+++ b/doc/后续工作20130921起/28分析软件后续工作和服务器站点【持续更新】.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>服务器站点列表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,12 +303,59 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>统一为类：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UserLogic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>用户查询：QueryUser()；获取单个用户：GetBySysNo()；启用：EnableUser()；禁用：DisableUser()；删除：DeleteUser()。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +405,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -492,6 +547,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,12 +573,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -835,22 +890,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="14"/>
-      <c r="J1" s="7" t="s">
+      <c r="H1" s="7"/>
+      <c r="J1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -894,7 +949,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -928,7 +983,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
@@ -1053,11 +1108,11 @@
       <c r="H8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:13" ht="27">
       <c r="A9" s="1">
@@ -1118,7 +1173,7 @@
       <c r="J10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="12" t="s">
         <v>48</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -1145,13 +1200,13 @@
       <c r="G11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="8" t="s">
         <v>67</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="13"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="1" t="s">
         <v>54</v>
       </c>
@@ -1182,12 +1237,12 @@
       <c r="J12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="11"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="27">
+    <row r="13" spans="1:13" ht="81">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1204,8 +1259,12 @@
       <c r="F13" s="1">
         <v>2</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="4"/>
+      <c r="G13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="27">
       <c r="A14" s="1">

</xml_diff>